<commit_message>
update readme and images
</commit_message>
<xml_diff>
--- a/data_demo/cal_parameters_demo.xlsx
+++ b/data_demo/cal_parameters_demo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\MATLAB\shadowtracking\data_demo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ljbak\My Drive\MATLAB\shadowtracking\data_demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51ABAF8-8BC0-40C8-A8CD-0C82C8E3D70A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B05E9A-6C49-4973-990E-3E5980496B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18432" windowHeight="12360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -201,12 +201,48 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -230,11 +266,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -552,213 +609,213 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="60">
+    <row r="1" spans="1:13" ht="41.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="11" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="10">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="6">
         <v>17</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="6">
         <v>10</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="4">
         <v>-17.5</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="4">
         <v>-11.5</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="8">
         <v>0.57999999999999996</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="8">
         <v>300</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="8">
         <v>5000</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="12">
         <v>73</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="12">
         <v>3950</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="12">
         <v>2050</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="12">
         <v>3761</v>
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="10">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="6">
         <v>16</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="6">
         <v>10</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="4">
         <v>-8.5</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="4">
         <v>-10.5</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="8">
         <v>0.57999999999999996</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="8">
         <v>300</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="8">
         <v>5000</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="12">
         <v>107</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="12">
         <v>3909</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="12">
         <v>2054</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="12">
         <v>3716</v>
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="10">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="6">
         <v>16</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="6">
         <v>5</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="4">
         <v>5.5</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="4">
         <v>-10.5</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="8">
         <v>0.57999999999999996</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="8">
         <v>300</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="8">
         <v>6000</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="12">
         <v>87</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="12">
         <v>3712</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="12">
         <v>1972</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="12">
         <v>3884</v>
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="10">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="6">
         <v>17</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="6">
         <v>10</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="4">
         <v>9.5</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="4">
         <v>-11.5</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="8">
         <v>0.57999999999999996</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="8">
         <v>300</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="8">
         <v>5000</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="12">
         <v>88</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="12">
         <v>3697</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="12">
         <v>2020</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="12">
         <v>3865</v>
       </c>
     </row>

</xml_diff>